<commit_message>
Refactoring of 2-nd lab
</commit_message>
<xml_diff>
--- a/Lab_2/Microsoft Excel Worksheet.xlsx
+++ b/Lab_2/Microsoft Excel Worksheet.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6905995C-0D1F-4361-BFE3-EB5DB24F03D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="5715" yWindow="2085" windowWidth="27870" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -89,7 +90,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -112,7 +112,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="be-BY"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -178,7 +178,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="be-BY"/>
+                <a:endParaRPr lang="ru-RU"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -191,7 +191,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -237,21 +236,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34300000000000003</c:v>
+                  <c:v>0.188</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.7029999999999998</c:v>
+                  <c:v>1.99</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.485999999999997</c:v>
+                  <c:v>25.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-359D-43DE-9F05-C2A5755BC217}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="ctr"/>
@@ -304,7 +308,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="be-BY"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1049825168"/>
@@ -360,7 +364,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="be-BY"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1049827344"/>
@@ -401,7 +405,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="be-BY"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -937,7 +941,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Диаграмма 3"/>
+        <xdr:cNvPr id="4" name="Диаграмма 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1031,6 +1041,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1066,6 +1093,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1241,11 +1285,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1311,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>3.1E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1275,7 +1319,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>0.34300000000000003</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1283,7 +1327,7 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>3.7029999999999998</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1291,7 +1335,7 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>43.485999999999997</v>
+        <v>25.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>